<commit_message>
Updated Operations Reimbursements.xlsx again
git-svn-id: svn+ssh://localhost/home/pcb/svn@321 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/Operations/accounts/Reimbursements/Operations Reimbursements.xlsx
+++ b/Operations/accounts/Reimbursements/Operations Reimbursements.xlsx
@@ -117,7 +117,7 @@
     <t>Alexis Shaw</t>
   </si>
   <si>
-    <t>Aiden Rhodes</t>
+    <t>Aiden Rohde</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>